<commit_message>
Update student, lecturer, groupStudent, topic controller and route
</commit_message>
<xml_diff>
--- a/public/uploads/lecturers.xlsx
+++ b/public/uploads/lecturers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vscode\manage-graduation-thesis-iuh-be\public\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC95B543-0EA2-4CD8-A525-BF1FA40D57DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F859BA9-89A4-4D27-AB18-422B67C5543B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FBCEDE1D-8498-4888-B650-4265EA4D3DD5}"/>
   </bookViews>
@@ -729,7 +729,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -765,7 +765,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="16">
-        <v>20001234</v>
+        <v>20011234</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
@@ -785,7 +785,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="8">
-        <v>20001235</v>
+        <v>20011235</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>6</v>
@@ -805,7 +805,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="8">
-        <v>20001236</v>
+        <v>20011236</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>9</v>
@@ -825,7 +825,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="16">
-        <v>20001237</v>
+        <v>20011237</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>12</v>
@@ -845,7 +845,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="8">
-        <v>20001238</v>
+        <v>20011238</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>15</v>
@@ -865,7 +865,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="8">
-        <v>20001239</v>
+        <v>20011239</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>42</v>
@@ -885,7 +885,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="16">
-        <v>20001240</v>
+        <v>20011240</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>20</v>
@@ -905,7 +905,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="8">
-        <v>20001241</v>
+        <v>20011241</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>23</v>
@@ -925,7 +925,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="8">
-        <v>20001242</v>
+        <v>20011242</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>26</v>
@@ -945,7 +945,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="16">
-        <v>20001243</v>
+        <v>20011243</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>29</v>
@@ -965,7 +965,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="8">
-        <v>20001254</v>
+        <v>20011254</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>32</v>
@@ -985,7 +985,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="8">
-        <v>20001255</v>
+        <v>20011255</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Update importStudent, importLecturer, getTermById
</commit_message>
<xml_diff>
--- a/public/uploads/lecturers.xlsx
+++ b/public/uploads/lecturers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vscode\manage-graduation-thesis-iuh-be\public\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F859BA9-89A4-4D27-AB18-422B67C5543B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357550D3-CBBD-4E6D-B720-C839E750B8E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FBCEDE1D-8498-4888-B650-4265EA4D3DD5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t>STT</t>
   </si>
@@ -168,13 +168,19 @@
   </si>
   <si>
     <t>Mã GV</t>
+  </si>
+  <si>
+    <t>0773070597</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Nhung</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,6 +214,12 @@
       <color rgb="FF0000FF"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -726,10 +738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F040A30-B09B-410E-B35F-FBC22D983D97}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1000,7 +1012,28 @@
         <v>37</v>
       </c>
     </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="8">
+        <v>20011256</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{4DFF2338-6610-4BBF-B200-B262CDF8ECBC}"/>
     <hyperlink ref="F3" r:id="rId2" xr:uid="{62954DCB-F82B-4DB0-9303-DD1AFB295E83}"/>
@@ -1014,6 +1047,7 @@
     <hyperlink ref="F11" r:id="rId10" xr:uid="{21197ADF-66FC-4B18-A5BB-9BE2D6589B58}"/>
     <hyperlink ref="F12" r:id="rId11" xr:uid="{D1FF9E60-E4C2-48A8-BFCD-2A4540B5C379}"/>
     <hyperlink ref="F13" r:id="rId12" xr:uid="{7B374CB6-8B2B-4BB7-9978-08B4F9A3AC66}"/>
+    <hyperlink ref="F14" r:id="rId13" xr:uid="{9B3C76A8-A353-40CD-88EC-9B6575698625}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feature: notification by id, by me, create all notification by term,add new lecturerTerm, fix: assign
</commit_message>
<xml_diff>
--- a/public/uploads/lecturers.xlsx
+++ b/public/uploads/lecturers.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vscode\manage-graduation-thesis-iuh-be\public\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coder\manage-graduation-thesis-iuh-be\public\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357550D3-CBBD-4E6D-B720-C839E750B8E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FBCEDE1D-8498-4888-B650-4265EA4D3DD5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
   <si>
     <t>STT</t>
   </si>
@@ -170,17 +169,47 @@
     <t>Mã GV</t>
   </si>
   <si>
-    <t>0773070597</t>
-  </si>
-  <si>
-    <t>Nguyễn Thị Nhung</t>
+    <t>0122002</t>
+  </si>
+  <si>
+    <t>01120050</t>
+  </si>
+  <si>
+    <t>01120013</t>
+  </si>
+  <si>
+    <t>01120034</t>
+  </si>
+  <si>
+    <t>01120012</t>
+  </si>
+  <si>
+    <t>01120014</t>
+  </si>
+  <si>
+    <t>06690007</t>
+  </si>
+  <si>
+    <t>06690051</t>
+  </si>
+  <si>
+    <t>01120016</t>
+  </si>
+  <si>
+    <t>01120049</t>
+  </si>
+  <si>
+    <t>01120009</t>
+  </si>
+  <si>
+    <t>01004004</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,8 +250,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -233,6 +274,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -353,7 +400,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -400,13 +447,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 5" xfId="1" xr:uid="{C3B7427E-7762-4811-8D28-EC0EE5894ABC}"/>
+    <cellStyle name="Normal 5" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -737,22 +787,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F040A30-B09B-410E-B35F-FBC22D983D97}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" customWidth="1"/>
-    <col min="3" max="4" width="25.44140625" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="30.88671875" customWidth="1"/>
+    <col min="1" max="2" width="8.8984375" customWidth="1"/>
+    <col min="3" max="4" width="25.3984375" customWidth="1"/>
+    <col min="5" max="5" width="18.296875" customWidth="1"/>
+    <col min="6" max="6" width="30.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="19.8" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -772,12 +822,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15.6">
       <c r="A2" s="12">
         <v>1</v>
       </c>
-      <c r="B2" s="16">
-        <v>20011234</v>
+      <c r="B2" s="17" t="s">
+        <v>47</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
@@ -792,12 +842,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15.6">
       <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="8">
-        <v>20011235</v>
+      <c r="B3" s="17" t="s">
+        <v>52</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>6</v>
@@ -812,12 +862,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15.6">
       <c r="A4" s="13">
         <v>3</v>
       </c>
-      <c r="B4" s="8">
-        <v>20011236</v>
+      <c r="B4" s="17" t="s">
+        <v>55</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>9</v>
@@ -832,12 +882,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15.6">
       <c r="A5" s="13">
         <v>4</v>
       </c>
-      <c r="B5" s="16">
-        <v>20011237</v>
+      <c r="B5" s="17" t="s">
+        <v>48</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>12</v>
@@ -852,12 +902,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="15.6">
       <c r="A6" s="13">
         <v>5</v>
       </c>
-      <c r="B6" s="8">
-        <v>20011238</v>
+      <c r="B6" s="17" t="s">
+        <v>54</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>15</v>
@@ -872,12 +922,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15.6">
       <c r="A7" s="13">
         <v>6</v>
       </c>
-      <c r="B7" s="8">
-        <v>20011239</v>
+      <c r="B7" s="17" t="s">
+        <v>45</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>42</v>
@@ -892,12 +942,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15.6">
       <c r="A8" s="13">
         <v>7</v>
       </c>
-      <c r="B8" s="16">
-        <v>20011240</v>
+      <c r="B8" s="17" t="s">
+        <v>46</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>20</v>
@@ -912,12 +962,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15.6">
       <c r="A9" s="13">
         <v>8</v>
       </c>
-      <c r="B9" s="8">
-        <v>20011241</v>
+      <c r="B9" s="17" t="s">
+        <v>50</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>23</v>
@@ -932,12 +982,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15.6">
       <c r="A10" s="13">
         <v>9</v>
       </c>
-      <c r="B10" s="8">
-        <v>20011242</v>
+      <c r="B10" s="17" t="s">
+        <v>53</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>26</v>
@@ -952,12 +1002,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15.6">
       <c r="A11" s="13">
         <v>10</v>
       </c>
-      <c r="B11" s="16">
-        <v>20011243</v>
+      <c r="B11" s="17" t="s">
+        <v>49</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>29</v>
@@ -972,12 +1022,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="15.6">
       <c r="A12" s="13">
         <v>11</v>
       </c>
-      <c r="B12" s="8">
-        <v>20011254</v>
+      <c r="B12" s="17" t="s">
+        <v>51</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>32</v>
@@ -992,12 +1042,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="15.6">
       <c r="A13" s="14">
         <v>12</v>
       </c>
-      <c r="B13" s="8">
-        <v>20011255</v>
+      <c r="B13" s="16" t="s">
+        <v>44</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>35</v>
@@ -1012,42 +1062,29 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="14">
-        <v>13</v>
-      </c>
-      <c r="B14" s="8">
-        <v>20011256</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>37</v>
-      </c>
+    <row r="14" spans="1:6">
+      <c r="A14" s="14"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{4DFF2338-6610-4BBF-B200-B262CDF8ECBC}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{62954DCB-F82B-4DB0-9303-DD1AFB295E83}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{B10F5AA1-199F-430E-9F72-6862CC49E4D3}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{1AF8B857-05AA-484E-A233-6BFB054EBB10}"/>
-    <hyperlink ref="F6" r:id="rId5" xr:uid="{C7D966C8-78E5-43F5-B9E6-4AF268507115}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{AFC43540-6050-4816-AB53-A8CE2850D1FB}"/>
-    <hyperlink ref="F8" r:id="rId7" xr:uid="{EA0DDF55-84E7-4AC5-9AAD-0A454A7B086D}"/>
-    <hyperlink ref="F9" r:id="rId8" xr:uid="{2E49BD3C-4F8B-4016-AB87-8D44E525CC74}"/>
-    <hyperlink ref="F10" r:id="rId9" xr:uid="{347FC70F-CA1E-4C8B-9313-3A1BC11BDCF5}"/>
-    <hyperlink ref="F11" r:id="rId10" xr:uid="{21197ADF-66FC-4B18-A5BB-9BE2D6589B58}"/>
-    <hyperlink ref="F12" r:id="rId11" xr:uid="{D1FF9E60-E4C2-48A8-BFCD-2A4540B5C379}"/>
-    <hyperlink ref="F13" r:id="rId12" xr:uid="{7B374CB6-8B2B-4BB7-9978-08B4F9A3AC66}"/>
-    <hyperlink ref="F14" r:id="rId13" xr:uid="{9B3C76A8-A353-40CD-88EC-9B6575698625}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F5" r:id="rId4"/>
+    <hyperlink ref="F6" r:id="rId5"/>
+    <hyperlink ref="F7" r:id="rId6"/>
+    <hyperlink ref="F8" r:id="rId7"/>
+    <hyperlink ref="F9" r:id="rId8"/>
+    <hyperlink ref="F10" r:id="rId9"/>
+    <hyperlink ref="F11" r:id="rId10"/>
+    <hyperlink ref="F12" r:id="rId11"/>
+    <hyperlink ref="F13" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>